<commit_message>
cambios finales pagina web 11:29
</commit_message>
<xml_diff>
--- a/HackProject/Archivos/Proveedores/ElCorral.xlsx
+++ b/HackProject/Archivos/Proveedores/ElCorral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuario\Desktop\Proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39EAF5A7-B9BD-49D5-A00E-0A9723FF05E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E744808-D9E7-44C7-875F-ED3F99703C04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590" xr2:uid="{8D6A3E8E-300A-4A3B-956C-D54DA149F6DD}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -453,7 +453,7 @@
         <v>10000</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>1250</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -464,7 +464,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -473,7 +473,7 @@
         <v>13000</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>1300</v>
       </c>
       <c r="F3">
         <v>13</v>
@@ -484,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -493,7 +493,7 @@
         <v>16000</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>1399</v>
       </c>
       <c r="F4">
         <v>30</v>

</xml_diff>